<commit_message>
added test on pac bayesian cut with fake complete Multilink dendogram
</commit_message>
<xml_diff>
--- a/data/dendogram.xlsx
+++ b/data/dendogram.xlsx
@@ -1,36 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allem\Desktop\IACV-Project\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FA2DEF2-824C-4322-B8B5-47996219F748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CC084BF-E67E-497E-AF08-6943BCAA4682}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Foglio1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -673,14 +652,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -691,7 +677,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -703,34 +696,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -757,116 +759,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -878,2476 +846,2501 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC826E47-96BA-4A22-96AC-F84789FBFE7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:C211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1">
         <v>121</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1">
         <v>113</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>114</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1">
         <v>42</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1">
         <v>119</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>120</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>199</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1">
         <v>50</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1">
         <v>57</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="1">
         <v>62</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>63</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="1">
         <v>21</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="1">
         <v>71</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>73</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="1">
         <v>35</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="1">
         <v>46</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="1">
         <v>161</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>162</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="1">
         <v>75</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>76</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="1">
         <v>45</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>244</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="1">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>11</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="1">
         <v>236</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>246</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="1">
         <v>106</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>107</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="1">
         <v>59</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>238</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="1">
         <v>47</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>248</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="1">
         <v>17</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>18</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="A25" s="1">
         <v>72</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>242</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+      <c r="A26" s="1">
         <v>105</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>251</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>24</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="A28" s="1">
         <v>249</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>250</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="A29" s="1">
         <v>168</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>169</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+      <c r="A30" s="1">
         <v>67</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>68</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="1">
         <v>112</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>232</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="1">
         <v>53</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>237</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="1">
         <v>26</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>27</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="1">
         <v>70</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>255</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+      <c r="A35" s="1">
         <v>54</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>55</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>243</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+      <c r="A37" s="1">
         <v>69</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>264</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+      <c r="A38" s="1">
         <v>49</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>253</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+      <c r="A39" s="1">
         <v>99</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>100</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+      <c r="A40" s="1">
         <v>20</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>241</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+      <c r="A41" s="1">
         <v>177</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>178</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+      <c r="A42" s="1">
         <v>254</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>270</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+      <c r="A43" s="1">
         <v>66</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>260</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+      <c r="A44" s="1">
         <v>258</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>272</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+      <c r="A45" s="1">
         <v>108</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>256</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+      <c r="A46" s="1">
         <v>267</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>273</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+      <c r="A47" s="1">
         <v>52</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>265</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+      <c r="A48" s="1">
         <v>268</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>277</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+      <c r="A49" s="1">
         <v>37</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>38</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+      <c r="A50" s="1">
         <v>64</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>239</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+      <c r="A51" s="1">
         <v>262</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>278</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+      <c r="A52" s="1">
         <v>4</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>240</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+      <c r="A53" s="1">
         <v>110</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>275</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+      <c r="A54" s="1">
         <v>40</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>41</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+      <c r="A55" s="1">
         <v>89</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>90</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+      <c r="A56" s="1">
         <v>1</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>282</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+      <c r="A57" s="1">
         <v>142</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>143</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+      <c r="A58" s="1">
         <v>279</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>284</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+      <c r="A59" s="1">
         <v>130</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>131</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+      <c r="A60" s="1">
         <v>257</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>263</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+      <c r="A61" s="1">
         <v>233</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>281</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+      <c r="A62" s="1">
         <v>78</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>80</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+      <c r="A63" s="1">
         <v>116</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>118</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+      <c r="A64" s="1">
         <v>77</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>247</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+      <c r="A65" s="1">
         <v>101</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>269</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+      <c r="A66" s="1">
         <v>28</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>290</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+      <c r="A67" s="1">
         <v>9</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>235</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
+      <c r="A68" s="1">
         <v>111</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>283</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
+      <c r="A69" s="1">
         <v>261</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>298</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+      <c r="A70" s="1">
         <v>86</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>87</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+      <c r="A71" s="1">
         <v>2</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>286</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
+      <c r="A72" s="1">
         <v>292</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>294</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
+      <c r="A73" s="1">
         <v>81</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>302</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
+      <c r="A74" s="1">
         <v>3</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>301</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+      <c r="A75" s="1">
         <v>274</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>296</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+      <c r="A76" s="1">
         <v>139</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>140</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
+      <c r="A77" s="1">
         <v>132</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>133</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
+      <c r="A78" s="1">
         <v>171</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>172</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
+      <c r="A79" s="1">
         <v>103</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>299</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
+      <c r="A80" s="1">
         <v>60</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>252</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
+      <c r="A81" s="1">
         <v>102</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>309</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
+      <c r="A82" s="1">
         <v>165</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>166</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
+      <c r="A83" s="1">
         <v>39</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>288</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
+      <c r="A84" s="1">
         <v>83</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>85</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
+      <c r="A85" s="1">
         <v>175</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>176</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
+      <c r="A86" s="1">
         <v>104</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>311</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
+      <c r="A87" s="1">
         <v>173</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>174</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
+      <c r="A88" s="1">
         <v>141</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>306</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
+      <c r="A89" s="1">
         <v>134</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>307</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
+      <c r="A90" s="1">
         <v>304</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>305</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
+      <c r="A91" s="1">
         <v>91</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>285</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
+      <c r="A92" s="1">
         <v>291</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>313</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
+      <c r="A93" s="1">
         <v>82</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>314</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
+      <c r="A94" s="1">
         <v>266</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>322</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
+      <c r="A95" s="1">
         <v>308</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>317</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
+      <c r="A96" s="1">
         <v>271</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>315</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
+      <c r="A97" s="1">
         <v>122</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>123</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
+      <c r="A98" s="1">
         <v>310</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>324</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
+      <c r="A99" s="1">
         <v>167</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
         <v>312</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
+      <c r="A100" s="1">
         <v>115</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
         <v>117</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
+      <c r="A101" s="1">
         <v>25</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
         <v>320</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
+      <c r="A102" s="1">
         <v>325</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
         <v>326</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
+      <c r="A103" s="1">
         <v>234</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="1">
         <v>293</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
+      <c r="A104" s="1">
         <v>61</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="1">
         <v>280</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
+      <c r="A105" s="1">
         <v>179</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="1">
         <v>231</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
+      <c r="A106" s="1">
         <v>30</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="1">
         <v>321</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
+      <c r="A107" s="1">
         <v>29</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="1">
         <v>331</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
+      <c r="A108" s="1">
         <v>316</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="1">
         <v>330</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
+      <c r="A109" s="1">
         <v>31</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="1">
         <v>328</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
+      <c r="A110" s="1">
         <v>155</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="1">
         <v>156</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
+      <c r="A111" s="1">
         <v>163</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="1">
         <v>245</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5">
+      <c r="A112" s="1">
         <v>33</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="1">
         <v>339</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5">
+      <c r="A113" s="1">
         <v>94</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="1">
         <v>95</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5">
+      <c r="A114" s="1">
         <v>276</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="1">
         <v>303</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5">
+      <c r="A115" s="1">
         <v>144</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="1">
         <v>145</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5">
+      <c r="A116" s="1">
         <v>109</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="1">
         <v>338</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5">
+      <c r="A117" s="1">
         <v>327</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="1">
         <v>335</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5">
+      <c r="A118" s="1">
         <v>332</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="1">
         <v>347</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="19.5">
+      <c r="A119" s="1">
         <v>79</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="1">
         <v>344</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="19.5">
+      <c r="A120" s="1">
         <v>334</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="1">
         <v>349</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="19.5">
+      <c r="A121" s="1">
         <v>336</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="1">
         <v>337</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="19.5">
+      <c r="A122" s="1">
         <v>259</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="1">
         <v>329</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="19.5">
+      <c r="A123" s="1">
         <v>342</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="1">
         <v>351</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5">
+      <c r="A124" s="1">
         <v>146</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="1">
         <v>345</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5">
+      <c r="A125" s="1">
         <v>226</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="1">
         <v>348</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5">
+      <c r="A126" s="1">
         <v>287</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="1">
         <v>318</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5">
+      <c r="A127" s="1">
         <v>124</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="1">
         <v>355</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5">
+      <c r="A128" s="1">
         <v>32</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="1">
         <v>353</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5">
+      <c r="A129" s="1">
         <v>170</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="1">
         <v>357</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5">
+      <c r="A130" s="1">
         <v>5</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="1">
         <v>297</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5">
+      <c r="A131" s="1">
         <v>333</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="1">
         <v>346</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5">
+      <c r="A132" s="1">
         <v>19</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="1">
         <v>358</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5">
+      <c r="A133" s="1">
         <v>360</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="1">
         <v>362</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5">
+      <c r="A134" s="1">
         <v>151</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="1">
         <v>152</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5">
+      <c r="A135" s="1">
         <v>97</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="1">
         <v>343</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5">
+      <c r="A136" s="1">
         <v>129</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="1">
         <v>289</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5">
+      <c r="A137" s="1">
         <v>354</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="1">
         <v>356</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="19.5">
+      <c r="A138" s="1">
         <v>138</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="1">
         <v>367</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5">
+      <c r="A139" s="1">
         <v>44</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="1">
         <v>363</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5">
+      <c r="A140" s="1">
         <v>56</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="1">
         <v>369</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5">
+      <c r="A141" s="1">
         <v>323</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="1">
         <v>350</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5">
+      <c r="A142" s="1">
         <v>160</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="1">
         <v>341</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5">
+      <c r="A143" s="1">
         <v>98</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="1">
         <v>295</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5">
+      <c r="A144" s="1">
         <v>125</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="1">
         <v>359</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5">
+      <c r="A145" s="1">
         <v>319</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="1">
         <v>366</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5">
+      <c r="A146" s="1">
         <v>93</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="1">
         <v>365</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5">
+      <c r="A147" s="1">
         <v>147</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="1">
         <v>368</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
+      <c r="A148" s="1">
         <v>150</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="1">
         <v>364</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
+      <c r="A149" s="1">
         <v>159</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="1">
         <v>372</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5">
+      <c r="A150" s="1">
         <v>157</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="1">
         <v>340</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5">
+      <c r="A151" s="1">
         <v>300</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="1">
         <v>371</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5">
+      <c r="A152" s="1">
         <v>148</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="1">
         <v>149</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
+      <c r="A153" s="1">
         <v>205</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="1">
         <v>206</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
+      <c r="A154" s="1">
         <v>373</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="1">
         <v>376</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
+      <c r="A155" s="1">
         <v>135</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="1">
         <v>375</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
+      <c r="A156" s="1">
         <v>352</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="1">
         <v>379</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
+      <c r="A157" s="1">
         <v>153</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="1">
         <v>378</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
+      <c r="A158" s="1">
         <v>128</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="1">
         <v>385</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
+      <c r="A159" s="1">
         <v>65</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="1">
         <v>381</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
+      <c r="A160" s="1">
         <v>154</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="1">
         <v>387</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
+      <c r="A161" s="1">
         <v>164</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="1">
         <v>386</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
+      <c r="A162" s="1">
         <v>220</v>
       </c>
-      <c r="B162">
+      <c r="B162" s="1">
         <v>221</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5">
+      <c r="A163" s="1">
         <v>137</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="1">
         <v>377</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
+      <c r="A164" s="1">
         <v>382</v>
       </c>
-      <c r="B164">
+      <c r="B164" s="1">
         <v>393</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5">
+      <c r="A165" s="1">
         <v>374</v>
       </c>
-      <c r="B165">
+      <c r="B165" s="1">
         <v>391</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5">
+      <c r="A166" s="1">
         <v>361</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="1">
         <v>384</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5">
+      <c r="A167" s="1">
         <v>158</v>
       </c>
-      <c r="B167">
+      <c r="B167" s="1">
         <v>380</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="19.5">
+      <c r="A168" s="1">
         <v>190</v>
       </c>
-      <c r="B168">
+      <c r="B168" s="1">
         <v>200</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
+      <c r="A169" s="1">
         <v>390</v>
       </c>
-      <c r="B169">
+      <c r="B169" s="1">
         <v>397</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
+      <c r="A170" s="1">
         <v>127</v>
       </c>
-      <c r="B170">
+      <c r="B170" s="1">
         <v>395</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
+      <c r="A171" s="1">
         <v>126</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="1">
         <v>388</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C171" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5">
+      <c r="A172" s="1">
         <v>204</v>
       </c>
-      <c r="B172">
+      <c r="B172" s="1">
         <v>207</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
+      <c r="A173" s="1">
         <v>88</v>
       </c>
-      <c r="B173">
+      <c r="B173" s="1">
         <v>389</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
+      <c r="A174" s="1">
         <v>74</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="1">
         <v>403</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
+      <c r="A175" s="1">
         <v>396</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="1">
         <v>404</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5">
+      <c r="A176" s="1">
         <v>400</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="1">
         <v>401</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5">
+      <c r="A177" s="1">
         <v>212</v>
       </c>
-      <c r="B177">
+      <c r="B177" s="1">
         <v>392</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="19.5">
+      <c r="A178" s="1">
         <v>394</v>
       </c>
-      <c r="B178">
+      <c r="B178" s="1">
         <v>406</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="19.5">
+      <c r="A179" s="1">
         <v>399</v>
       </c>
-      <c r="B179">
+      <c r="B179" s="1">
         <v>408</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="19.5">
+      <c r="A180" s="1">
         <v>15</v>
       </c>
-      <c r="B180">
+      <c r="B180" s="1">
         <v>370</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="19.5">
+      <c r="A181" s="1">
         <v>224</v>
       </c>
-      <c r="B181">
+      <c r="B181" s="1">
         <v>402</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="19.5">
+      <c r="A182" s="1">
         <v>92</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="1">
         <v>405</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="19.5">
+      <c r="A183" s="1">
         <v>185</v>
       </c>
-      <c r="B183">
+      <c r="B183" s="1">
         <v>214</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="19.5">
+      <c r="A184" s="1">
         <v>191</v>
       </c>
-      <c r="B184">
+      <c r="B184" s="1">
         <v>398</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5">
+      <c r="A185" s="1">
         <v>136</v>
       </c>
-      <c r="B185">
+      <c r="B185" s="1">
         <v>219</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="19.5">
+      <c r="A186" s="1">
         <v>198</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="1">
         <v>211</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="19.5">
+      <c r="A187" s="1">
         <v>183</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="1">
         <v>196</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="19.5">
+      <c r="A188" s="1">
         <v>187</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="1">
         <v>197</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="19.5">
+      <c r="A189" s="1">
         <v>192</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="1">
         <v>416</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="19.5">
+      <c r="A190" s="1">
         <v>193</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="1">
         <v>215</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C190" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="19.5">
+      <c r="A191" s="1">
         <v>216</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="1">
         <v>415</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="19.5">
+      <c r="A192" s="1">
         <v>222</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="1">
         <v>223</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="19.5">
+      <c r="A193" s="1">
         <v>228</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="1">
         <v>422</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C193" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="19.5">
+      <c r="A194" s="1">
         <v>409</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="1">
         <v>421</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="19.5">
+      <c r="A195" s="1">
         <v>181</v>
       </c>
-      <c r="B195">
+      <c r="B195" s="1">
         <v>194</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5">
+      <c r="A196" s="1">
         <v>182</v>
       </c>
-      <c r="B196">
+      <c r="B196" s="1">
         <v>420</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="19.5">
+      <c r="A197" s="1">
         <v>186</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="1">
         <v>189</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="19.5">
+      <c r="A198" s="1">
         <v>96</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="1">
         <v>413</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="19.5">
+      <c r="A199" s="1">
         <v>84</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="1">
         <v>428</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200">
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="19.5">
+      <c r="A200" s="1">
         <v>201</v>
       </c>
-      <c r="B200">
+      <c r="B200" s="1">
         <v>208</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C200" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201">
+    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="19.5">
+      <c r="A201" s="1">
         <v>202</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="1">
         <v>230</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202">
+    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="19.5">
+      <c r="A202" s="1">
         <v>203</v>
       </c>
-      <c r="B202">
+      <c r="B202" s="1">
         <v>225</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C202" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203">
+    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="19.5">
+      <c r="A203" s="1">
         <v>213</v>
       </c>
-      <c r="B203">
+      <c r="B203" s="1">
         <v>432</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C203" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A204">
+    <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="19.5">
+      <c r="A204" s="1">
         <v>218</v>
       </c>
-      <c r="B204">
+      <c r="B204" s="1">
         <v>227</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C204" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A205">
+    <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="19.5">
+      <c r="A205" s="1">
         <v>210</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="1">
         <v>417</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C205" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206">
+    <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="19.5">
+      <c r="A206" s="1">
         <v>407</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="1">
         <v>427</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C206" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207">
+    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="19.5">
+      <c r="A207" s="1">
         <v>414</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="1">
         <v>423</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A208">
+    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="19.5">
+      <c r="A208" s="1">
         <v>184</v>
       </c>
-      <c r="B208">
+      <c r="B208" s="1">
         <v>188</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A209">
+    <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="19.5">
+      <c r="A209" s="1">
         <v>426</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="1">
         <v>433</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A210">
+    <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="19.5">
+      <c r="A210" s="1">
         <v>217</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="1">
         <v>229</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211">
+    <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="19.5">
+      <c r="A211" s="1">
         <v>209</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="1">
         <v>418</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C211" s="2" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>